<commit_message>
nmv 13 06 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF72188E-2625-41ED-98C5-2B3FFD894823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1960DE-A7FB-4FFB-BCD5-6ECE5BC58823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 5.7" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 5.7'!$A$1:$V$2583</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6657" uniqueCount="1719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6658" uniqueCount="1719">
   <si>
     <t>Passage</t>
   </si>
@@ -5377,7 +5369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5532,6 +5524,18 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5815,10 +5819,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2436" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A2583" sqref="A2583"/>
+      <selection pane="bottomLeft" activeCell="V2525" sqref="V2525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -11891,18 +11895,18 @@
         <f t="shared" si="9"/>
         <v>148</v>
       </c>
-      <c r="N149" s="35" t="s">
+      <c r="N149" s="53" t="s">
         <v>566</v>
       </c>
-      <c r="O149" s="7"/>
-      <c r="P149" s="8" t="s">
+      <c r="O149" s="54"/>
+      <c r="P149" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="Q149" s="8"/>
-      <c r="R149" s="8"/>
-      <c r="S149" s="8"/>
-      <c r="T149" s="8"/>
-      <c r="U149" s="8"/>
+      <c r="Q149" s="55"/>
+      <c r="R149" s="55"/>
+      <c r="S149" s="55"/>
+      <c r="T149" s="55"/>
+      <c r="U149" s="55"/>
       <c r="V149" s="35" t="s">
         <v>1618</v>
       </c>
@@ -33932,7 +33936,9 @@
       <c r="N783" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="O783" s="7"/>
+      <c r="O783" s="50" t="s">
+        <v>81</v>
+      </c>
       <c r="P783" s="8"/>
       <c r="Q783" s="8"/>
       <c r="R783" s="8"/>
@@ -46178,18 +46184,19 @@
         <f t="shared" si="57"/>
         <v>345</v>
       </c>
-      <c r="N1172" s="35" t="s">
+      <c r="N1172" s="56" t="s">
         <v>770</v>
       </c>
-      <c r="O1172" s="8"/>
-      <c r="P1172" s="8" t="s">
+      <c r="O1172" s="52"/>
+      <c r="P1172" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="Q1172" s="8"/>
-      <c r="R1172" s="8"/>
-      <c r="S1172" s="8"/>
-      <c r="T1172" s="8"/>
-      <c r="V1172" s="35" t="s">
+      <c r="Q1172" s="52"/>
+      <c r="R1172" s="52"/>
+      <c r="S1172" s="52"/>
+      <c r="T1172" s="52"/>
+      <c r="U1172" s="52"/>
+      <c r="V1172" s="56" t="s">
         <v>1647</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nmv 23 07 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5C8F3B-E75E-4A4F-AC62-B34714828F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485A489-5C4E-42EE-88C9-9A28B70BD42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6668" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6667" uniqueCount="1721">
   <si>
     <t>Passage</t>
   </si>
@@ -5181,9 +5181,6 @@
     <t>uda~g#</t>
   </si>
   <si>
-    <t>upAyA ~jcitIByAm</t>
-  </si>
-  <si>
     <t>gRuhNAmyagre agre - alopam</t>
   </si>
   <si>
@@ -5191,6 +5188,9 @@
   </si>
   <si>
     <t>rAyo &amp;gnim - lopam</t>
+  </si>
+  <si>
+    <t>upAya ~jcitIByAm</t>
   </si>
 </sst>
 </file>
@@ -5393,7 +5393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5558,9 +5558,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5570,13 +5567,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5861,10 +5855,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2038" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2576" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2045" sqref="N2045"/>
+      <selection pane="bottomLeft" activeCell="N2508" sqref="N2507:N2508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -35901,7 +35895,7 @@
         <f t="shared" si="42"/>
         <v>17</v>
       </c>
-      <c r="N844" s="35" t="s">
+      <c r="N844" s="52" t="s">
         <v>288</v>
       </c>
       <c r="O844" s="8" t="s">
@@ -35934,7 +35928,7 @@
         <f t="shared" si="42"/>
         <v>18</v>
       </c>
-      <c r="N845" s="35" t="s">
+      <c r="N845" s="52" t="s">
         <v>630</v>
       </c>
       <c r="O845" s="8"/>
@@ -45415,7 +45409,7 @@
     </row>
     <row r="1147" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1147" s="55" t="s">
-        <v>1717</v>
+        <v>1720</v>
       </c>
       <c r="H1147" s="42" t="s">
         <v>108</v>
@@ -61361,46 +61355,43 @@
       <c r="V1659" s="35"/>
     </row>
     <row r="1660" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="H1660" s="56" t="s">
+      <c r="H1660" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="I1660" s="57" t="s">
+      <c r="I1660" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J1660" s="58">
+      <c r="J1660" s="9">
         <v>33</v>
       </c>
-      <c r="K1660" s="57">
+      <c r="K1660" s="38">
         <f t="shared" si="76"/>
         <v>1659</v>
       </c>
-      <c r="L1660" s="57">
+      <c r="L1660" s="38">
         <f t="shared" si="77"/>
         <v>21</v>
       </c>
-      <c r="M1660" s="57">
+      <c r="M1660" s="38">
         <f t="shared" si="78"/>
         <v>21</v>
       </c>
-      <c r="N1660" s="59" t="s">
+      <c r="N1660" s="35" t="s">
         <v>906</v>
       </c>
-      <c r="O1660" s="60" t="s">
+      <c r="O1660" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P1660" s="60" t="s">
+      <c r="P1660" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q1660" s="61"/>
-      <c r="R1660" s="61"/>
-      <c r="S1660" s="60" t="s">
+      <c r="S1660" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="T1660" s="60" t="s">
+      <c r="T1660" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="U1660" s="60"/>
-      <c r="V1660" s="59" t="s">
+      <c r="V1660" s="35" t="s">
         <v>1462</v>
       </c>
     </row>
@@ -65174,7 +65165,7 @@
     </row>
     <row r="1808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1808" s="8" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="G1808" s="46" t="s">
         <v>153</v>
@@ -65203,14 +65194,14 @@
       <c r="N1808" s="54" t="s">
         <v>582</v>
       </c>
-      <c r="U1808" s="62" t="s">
+      <c r="U1808" s="55" t="s">
         <v>128</v>
       </c>
       <c r="V1808" s="35"/>
     </row>
     <row r="1809" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1809" s="8" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="G1809" s="46" t="s">
         <v>153</v>
@@ -65246,7 +65237,7 @@
     </row>
     <row r="1810" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1810" s="8" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="G1810" s="46" t="s">
         <v>153</v>
@@ -66742,27 +66733,33 @@
       </c>
     </row>
     <row r="1866" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1866" s="38" t="s">
+      <c r="I1866" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="J1866" s="9">
+      <c r="J1866" s="57">
         <v>37</v>
       </c>
-      <c r="K1866" s="38">
+      <c r="K1866" s="56">
         <f t="shared" si="88"/>
         <v>1865</v>
       </c>
-      <c r="L1866" s="38">
+      <c r="L1866" s="56">
         <f t="shared" si="89"/>
         <v>11</v>
       </c>
-      <c r="M1866" s="38">
+      <c r="M1866" s="56">
         <f t="shared" si="90"/>
         <v>61</v>
       </c>
-      <c r="N1866" s="35" t="s">
+      <c r="N1866" s="58" t="s">
         <v>620</v>
       </c>
+      <c r="O1866" s="59"/>
+      <c r="P1866" s="60"/>
+      <c r="Q1866" s="60"/>
+      <c r="R1866" s="60"/>
+      <c r="S1866" s="60"/>
+      <c r="T1866" s="60"/>
       <c r="V1866" s="35"/>
     </row>
     <row r="1867" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66863,7 +66860,7 @@
     </row>
     <row r="1871" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1871" s="8" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="I1871" s="38" t="s">
         <v>56</v>
@@ -66893,7 +66890,7 @@
     </row>
     <row r="1872" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1872" s="8" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="I1872" s="38" t="s">
         <v>56</v>
@@ -66921,10 +66918,7 @@
       </c>
       <c r="V1872" s="35"/>
     </row>
-    <row r="1873" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1873" s="8" t="s">
-        <v>1720</v>
-      </c>
+    <row r="1873" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1873" s="38" t="s">
         <v>56</v>
       </c>
@@ -66948,7 +66942,7 @@
       </c>
       <c r="V1873" s="35"/>
     </row>
-    <row r="1874" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1874" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1874" s="38" t="s">
         <v>56</v>
       </c>
@@ -66972,7 +66966,7 @@
       </c>
       <c r="V1874" s="35"/>
     </row>
-    <row r="1875" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1875" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1875" s="38" t="s">
         <v>56</v>
       </c>
@@ -66996,7 +66990,7 @@
       </c>
       <c r="V1875" s="35"/>
     </row>
-    <row r="1876" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1876" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1876" s="38" t="s">
         <v>56</v>
       </c>
@@ -67020,7 +67014,7 @@
       </c>
       <c r="V1876" s="35"/>
     </row>
-    <row r="1877" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1877" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1877" s="38" t="s">
         <v>56</v>
       </c>
@@ -67044,7 +67038,7 @@
       </c>
       <c r="V1877" s="35"/>
     </row>
-    <row r="1878" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1878" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1878" s="38" t="s">
         <v>56</v>
       </c>
@@ -67068,7 +67062,7 @@
       </c>
       <c r="V1878" s="35"/>
     </row>
-    <row r="1879" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1879" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1879" s="38" t="s">
         <v>56</v>
       </c>
@@ -67092,7 +67086,7 @@
       </c>
       <c r="V1879" s="35"/>
     </row>
-    <row r="1880" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1880" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1880" s="38" t="s">
         <v>56</v>
       </c>
@@ -67116,7 +67110,7 @@
       </c>
       <c r="V1880" s="35"/>
     </row>
-    <row r="1881" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1881" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1881" s="38" t="s">
         <v>56</v>
       </c>
@@ -67140,7 +67134,7 @@
       </c>
       <c r="V1881" s="35"/>
     </row>
-    <row r="1882" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1882" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1882" s="38" t="s">
         <v>56</v>
       </c>
@@ -67164,7 +67158,7 @@
       </c>
       <c r="V1882" s="35"/>
     </row>
-    <row r="1883" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1883" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1883" s="38" t="s">
         <v>56</v>
       </c>
@@ -67191,7 +67185,7 @@
       </c>
       <c r="V1883" s="35"/>
     </row>
-    <row r="1884" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1884" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1884" s="38" t="s">
         <v>56</v>
       </c>
@@ -67215,7 +67209,7 @@
       </c>
       <c r="V1884" s="35"/>
     </row>
-    <row r="1885" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1885" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1885" s="38" t="s">
         <v>56</v>
       </c>
@@ -67244,7 +67238,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="1886" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1886" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1886" s="38" t="s">
         <v>56</v>
       </c>
@@ -67268,7 +67262,7 @@
       </c>
       <c r="V1886" s="35"/>
     </row>
-    <row r="1887" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1887" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1887" s="43" t="s">
         <v>137</v>
       </c>
@@ -67295,7 +67289,7 @@
       </c>
       <c r="V1887" s="35"/>
     </row>
-    <row r="1888" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1888" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1888" s="43" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
nmv 02 08 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE76AB71-76A2-4B06-AC0B-6D712041E855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F4422-4BEA-4779-9749-7983C631008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6667" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="1721">
   <si>
     <t>Passage</t>
   </si>
@@ -5843,10 +5843,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1646" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1648" sqref="V1648"/>
+      <selection pane="bottomLeft" activeCell="U239" sqref="U239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -15187,9 +15187,7 @@
       <c r="R239" s="8"/>
       <c r="S239" s="8"/>
       <c r="T239" s="8"/>
-      <c r="U239" s="8" t="s">
-        <v>128</v>
-      </c>
+      <c r="U239" s="8"/>
       <c r="V239" s="35"/>
     </row>
     <row r="240" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 05 08 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F4422-4BEA-4779-9749-7983C631008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE6F50D-F542-49A5-9A8F-63264AEC9ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6665" uniqueCount="1721">
   <si>
     <t>Passage</t>
   </si>
@@ -4098,9 +4098,6 @@
     <t>yatkA#maq itiq yat - kAqmaqH</t>
   </si>
   <si>
-    <t>eqte iti# eqte</t>
-  </si>
-  <si>
     <t>SaqtaqruqdrIyaqmiti# Sata - ruqdrIya$m</t>
   </si>
   <si>
@@ -5191,6 +5188,9 @@
   </si>
   <si>
     <t>jAqtaqveqdaqH</t>
+  </si>
+  <si>
+    <t>eqte ityeqte</t>
   </si>
 </sst>
 </file>
@@ -5843,10 +5843,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U239" sqref="U239"/>
+      <selection pane="bottomLeft" activeCell="U553" sqref="U553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6483,7 +6483,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>78</v>
@@ -11932,7 +11932,7 @@
       <c r="T149" s="8"/>
       <c r="U149" s="8"/>
       <c r="V149" s="35" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="150" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12104,7 +12104,7 @@
         <v>119</v>
       </c>
       <c r="T154" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="U154" s="8"/>
       <c r="V154" s="35"/>
@@ -12200,7 +12200,7 @@
         <v>8</v>
       </c>
       <c r="N157" s="35" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="O157" s="8" t="s">
         <v>78</v>
@@ -12214,7 +12214,7 @@
       <c r="T157" s="8"/>
       <c r="U157" s="8"/>
       <c r="V157" s="35" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="158" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12518,7 +12518,7 @@
         <v>17</v>
       </c>
       <c r="N166" s="35" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="O166" s="7"/>
       <c r="P166" s="8" t="s">
@@ -12530,7 +12530,7 @@
       <c r="T166" s="8"/>
       <c r="U166" s="8"/>
       <c r="V166" s="35" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="167" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13227,7 +13227,7 @@
         <v>36</v>
       </c>
       <c r="N185" s="35" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="O185" s="7"/>
       <c r="P185" s="8" t="s">
@@ -13239,7 +13239,7 @@
       <c r="T185" s="8"/>
       <c r="U185" s="8"/>
       <c r="V185" s="35" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="186" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13445,7 +13445,7 @@
         <v>42</v>
       </c>
       <c r="N191" s="35" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="O191" s="8" t="s">
         <v>78</v>
@@ -13459,7 +13459,7 @@
       <c r="T191" s="8"/>
       <c r="U191" s="8"/>
       <c r="V191" s="35" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="192" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13699,7 +13699,7 @@
         <v>49</v>
       </c>
       <c r="N198" s="35" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="O198" s="7"/>
       <c r="P198" s="8" t="s">
@@ -13711,7 +13711,7 @@
       <c r="T198" s="8"/>
       <c r="U198" s="8"/>
       <c r="V198" s="35" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="199" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14933,7 +14933,7 @@
         <v>83</v>
       </c>
       <c r="N232" s="36" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="O232" s="8" t="s">
         <v>78</v>
@@ -15107,7 +15107,7 @@
         <v>88</v>
       </c>
       <c r="N237" s="35" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="O237" s="7"/>
       <c r="P237" s="8" t="s">
@@ -15119,7 +15119,7 @@
       <c r="T237" s="8"/>
       <c r="U237" s="8"/>
       <c r="V237" s="35" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="238" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15387,7 +15387,7 @@
         <v>96</v>
       </c>
       <c r="N245" s="35" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="O245" s="7"/>
       <c r="P245" s="8" t="s">
@@ -15399,7 +15399,7 @@
       <c r="T245" s="8"/>
       <c r="U245" s="8"/>
       <c r="V245" s="35" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="246" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15805,7 +15805,7 @@
         <v>108</v>
       </c>
       <c r="N257" s="36" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="O257" s="8" t="s">
         <v>78</v>
@@ -16419,7 +16419,7 @@
         <v>125</v>
       </c>
       <c r="N274" s="35" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="O274" s="8" t="s">
         <v>78</v>
@@ -16433,7 +16433,7 @@
       <c r="T274" s="8"/>
       <c r="U274" s="8"/>
       <c r="V274" s="35" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="275" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -16795,7 +16795,7 @@
         <v>135</v>
       </c>
       <c r="N284" s="35" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="O284" s="7"/>
       <c r="P284" s="8" t="s">
@@ -16807,7 +16807,7 @@
       <c r="T284" s="8"/>
       <c r="U284" s="8"/>
       <c r="V284" s="35" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="285" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17050,7 +17050,7 @@
         <v>142</v>
       </c>
       <c r="N291" s="35" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="O291" s="8" t="s">
         <v>78</v>
@@ -17064,7 +17064,7 @@
       <c r="T291" s="8"/>
       <c r="U291" s="8"/>
       <c r="V291" s="35" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="292" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17479,7 +17479,7 @@
         <v>154</v>
       </c>
       <c r="N303" s="35" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="O303" s="7"/>
       <c r="P303" s="8" t="s">
@@ -17491,7 +17491,7 @@
       <c r="T303" s="8"/>
       <c r="U303" s="8"/>
       <c r="V303" s="35" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="304" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17823,7 +17823,7 @@
         <v>164</v>
       </c>
       <c r="N313" s="35" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="O313" s="7"/>
       <c r="P313" s="8" t="s">
@@ -17837,7 +17837,7 @@
         <v>129</v>
       </c>
       <c r="V313" s="35" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="314" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18087,7 +18087,7 @@
       <c r="T320" s="8"/>
       <c r="U320" s="8"/>
       <c r="V320" s="35" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="321" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18297,7 +18297,7 @@
         <v>177</v>
       </c>
       <c r="N326" s="35" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="O326" s="7"/>
       <c r="P326" s="8" t="s">
@@ -18309,7 +18309,7 @@
       <c r="T326" s="8"/>
       <c r="U326" s="8"/>
       <c r="V326" s="35" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="327" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18589,7 +18589,7 @@
       <c r="T334" s="8"/>
       <c r="U334" s="8"/>
       <c r="V334" s="35" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="335" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18971,7 +18971,7 @@
       <c r="T345" s="8"/>
       <c r="U345" s="8"/>
       <c r="V345" s="35" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="346" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19313,7 +19313,7 @@
         <v>206</v>
       </c>
       <c r="N355" s="35" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="O355" s="7"/>
       <c r="P355" s="8" t="s">
@@ -19325,7 +19325,7 @@
       <c r="T355" s="8"/>
       <c r="U355" s="8"/>
       <c r="V355" s="35" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="356" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20383,10 +20383,10 @@
       <c r="Q385" s="8"/>
       <c r="R385" s="8"/>
       <c r="S385" s="8" t="s">
+        <v>1682</v>
+      </c>
+      <c r="T385" s="8" t="s">
         <v>1683</v>
-      </c>
-      <c r="T385" s="8" t="s">
-        <v>1684</v>
       </c>
       <c r="U385" s="8"/>
       <c r="V385" s="35"/>
@@ -21071,7 +21071,7 @@
         <v>255</v>
       </c>
       <c r="N404" s="36" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="O404" s="8" t="s">
         <v>78</v>
@@ -21771,7 +21771,7 @@
         <v>275</v>
       </c>
       <c r="N424" s="35" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="O424" s="8" t="s">
         <v>78</v>
@@ -21785,7 +21785,7 @@
       <c r="T424" s="8"/>
       <c r="U424" s="8"/>
       <c r="V424" s="35" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="425" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22021,7 +22021,7 @@
         <v>7</v>
       </c>
       <c r="N431" s="35" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="O431" s="8" t="s">
         <v>78</v>
@@ -22035,7 +22035,7 @@
       <c r="T431" s="8"/>
       <c r="U431" s="8"/>
       <c r="V431" s="35" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="432" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22449,7 +22449,7 @@
         <v>19</v>
       </c>
       <c r="N443" s="35" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="O443" s="7"/>
       <c r="P443" s="8" t="s">
@@ -22461,7 +22461,7 @@
       <c r="T443" s="8"/>
       <c r="U443" s="8"/>
       <c r="V443" s="35" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="444" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22783,7 +22783,7 @@
         <v>106</v>
       </c>
       <c r="T452" s="8" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="U452" s="8"/>
       <c r="V452" s="35"/>
@@ -24020,7 +24020,7 @@
         <v>63</v>
       </c>
       <c r="N487" s="35" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="O487" s="7"/>
       <c r="P487" s="8" t="s">
@@ -24032,7 +24032,7 @@
       <c r="T487" s="8"/>
       <c r="U487" s="8"/>
       <c r="V487" s="35" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="488" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24162,7 +24162,7 @@
         <v>67</v>
       </c>
       <c r="N491" s="35" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="O491" s="7"/>
       <c r="P491" s="8" t="s">
@@ -24174,7 +24174,7 @@
       <c r="T491" s="8"/>
       <c r="U491" s="8"/>
       <c r="V491" s="35" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="492" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25964,8 +25964,8 @@
       <c r="S542" s="8"/>
       <c r="T542" s="8"/>
       <c r="U542" s="8"/>
-      <c r="V542" s="35" t="s">
-        <v>1356</v>
+      <c r="V542" s="36" t="s">
+        <v>1720</v>
       </c>
     </row>
     <row r="543" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26207,7 +26207,7 @@
       <c r="T549" s="8"/>
       <c r="U549" s="8"/>
       <c r="V549" s="35" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="550" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26343,9 +26343,7 @@
       <c r="R553" s="8"/>
       <c r="S553" s="8"/>
       <c r="T553" s="8"/>
-      <c r="U553" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="U553" s="8"/>
       <c r="V553" s="35"/>
     </row>
     <row r="554" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27100,7 +27098,7 @@
       <c r="T575" s="8"/>
       <c r="U575" s="8"/>
       <c r="V575" s="35" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="576" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27344,7 +27342,7 @@
       <c r="T582" s="8"/>
       <c r="U582" s="8"/>
       <c r="V582" s="35" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="583" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27380,7 +27378,7 @@
         <v>106</v>
       </c>
       <c r="T583" s="8" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="U583" s="8"/>
       <c r="V583" s="35"/>
@@ -27408,7 +27406,7 @@
         <v>160</v>
       </c>
       <c r="N584" s="35" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="O584" s="8" t="s">
         <v>78</v>
@@ -27420,7 +27418,7 @@
       <c r="T584" s="8"/>
       <c r="U584" s="8"/>
       <c r="V584" s="35" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="585" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28308,10 +28306,10 @@
       <c r="Q610" s="8"/>
       <c r="R610" s="8"/>
       <c r="S610" s="8" t="s">
+        <v>1686</v>
+      </c>
+      <c r="T610" s="8" t="s">
         <v>1687</v>
-      </c>
-      <c r="T610" s="8" t="s">
-        <v>1688</v>
       </c>
       <c r="U610" s="8"/>
       <c r="V610" s="35"/>
@@ -28627,7 +28625,7 @@
     </row>
     <row r="620" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A620" s="8" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B620" s="45"/>
       <c r="D620" s="17"/>
@@ -28662,7 +28660,7 @@
       <c r="T620" s="8"/>
       <c r="U620" s="8"/>
       <c r="V620" s="35" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="621" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29060,7 +29058,7 @@
       <c r="T631" s="14"/>
       <c r="U631" s="14"/>
       <c r="V631" s="35" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="632" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29086,7 +29084,7 @@
         <v>208</v>
       </c>
       <c r="N632" s="36" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="O632" s="8" t="s">
         <v>78</v>
@@ -29098,7 +29096,7 @@
       <c r="T632" s="8"/>
       <c r="U632" s="8"/>
       <c r="V632" s="36" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29724,7 +29722,7 @@
       <c r="T650" s="8"/>
       <c r="U650" s="8"/>
       <c r="V650" s="35" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="651" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29763,7 +29761,7 @@
       <c r="T651" s="8"/>
       <c r="U651" s="8"/>
       <c r="V651" s="36" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="652" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29985,7 +29983,7 @@
       <c r="T657" s="8"/>
       <c r="U657" s="8"/>
       <c r="V657" s="35" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="658" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -30419,7 +30417,7 @@
       <c r="S670" s="8"/>
       <c r="T670" s="8"/>
       <c r="V670" s="35" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="671" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30542,7 +30540,7 @@
       <c r="S674" s="8"/>
       <c r="T674" s="8"/>
       <c r="V674" s="35" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30728,7 +30726,7 @@
       <c r="S680" s="8"/>
       <c r="T680" s="8"/>
       <c r="V680" s="35" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="681" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31488,7 +31486,7 @@
       <c r="S705" s="8"/>
       <c r="T705" s="8"/>
       <c r="V705" s="35" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="706" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31559,7 +31557,7 @@
     </row>
     <row r="708" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A708" s="8" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="G708" s="46" t="s">
         <v>152</v>
@@ -31598,7 +31596,7 @@
     </row>
     <row r="709" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A709" s="8" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="G709" s="46" t="s">
         <v>152</v>
@@ -31672,7 +31670,7 @@
       <c r="S710" s="8"/>
       <c r="T710" s="8"/>
       <c r="V710" s="35" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="711" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32445,7 +32443,7 @@
       <c r="S735" s="8"/>
       <c r="T735" s="8"/>
       <c r="V735" s="35" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="736" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32482,7 +32480,7 @@
       <c r="S736" s="8"/>
       <c r="T736" s="8"/>
       <c r="V736" s="35" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="737" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32587,7 +32585,7 @@
       <c r="S739" s="8"/>
       <c r="T739" s="8"/>
       <c r="V739" s="35" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="740" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32711,7 +32709,7 @@
       <c r="S743" s="8"/>
       <c r="T743" s="8"/>
       <c r="V743" s="35" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="744" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32775,7 +32773,7 @@
       <c r="S745" s="8"/>
       <c r="T745" s="8"/>
       <c r="V745" s="35" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="746" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32798,7 +32796,7 @@
         <v>322</v>
       </c>
       <c r="N746" s="35" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="O746" s="7"/>
       <c r="P746" s="8" t="s">
@@ -32812,7 +32810,7 @@
         <v>129</v>
       </c>
       <c r="V746" s="35" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="747" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33077,7 +33075,7 @@
         <v>331</v>
       </c>
       <c r="N755" s="35" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="O755" s="8" t="s">
         <v>78</v>
@@ -33090,7 +33088,7 @@
       <c r="S755" s="8"/>
       <c r="T755" s="8"/>
       <c r="V755" s="35" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="756" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33453,7 +33451,7 @@
         <v>343</v>
       </c>
       <c r="N767" s="35" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="O767" s="7"/>
       <c r="P767" s="8" t="s">
@@ -33464,7 +33462,7 @@
       <c r="S767" s="8"/>
       <c r="T767" s="8"/>
       <c r="V767" s="35" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="768" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33528,7 +33526,7 @@
       <c r="S769" s="8"/>
       <c r="T769" s="8"/>
       <c r="V769" s="35" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="770" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33623,7 +33621,7 @@
       <c r="S772" s="8"/>
       <c r="T772" s="8"/>
       <c r="V772" s="35" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="773" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33710,7 +33708,7 @@
         <v>351</v>
       </c>
       <c r="N775" s="36" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="O775" s="8" t="s">
         <v>78</v>
@@ -33723,7 +33721,7 @@
       <c r="S775" s="8"/>
       <c r="T775" s="8"/>
       <c r="V775" s="35" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="776" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33817,7 +33815,7 @@
       <c r="S778" s="8"/>
       <c r="T778" s="8"/>
       <c r="V778" s="35" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="779" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34024,7 +34022,7 @@
         <v>361</v>
       </c>
       <c r="N785" s="35" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="O785" s="7"/>
       <c r="P785" s="8" t="s">
@@ -34035,7 +34033,7 @@
       <c r="S785" s="8"/>
       <c r="T785" s="8"/>
       <c r="V785" s="35" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="786" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34072,7 +34070,7 @@
       <c r="S786" s="8"/>
       <c r="T786" s="8"/>
       <c r="V786" s="35" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="787" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34339,7 +34337,7 @@
       <c r="S794" s="8"/>
       <c r="T794" s="8"/>
       <c r="V794" s="35" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="795" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34392,7 +34390,7 @@
         <v>372</v>
       </c>
       <c r="N796" s="35" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="O796" s="7"/>
       <c r="P796" s="8" t="s">
@@ -34406,7 +34404,7 @@
         <v>129</v>
       </c>
       <c r="V796" s="35" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="797" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34470,7 +34468,7 @@
       <c r="S798" s="8"/>
       <c r="T798" s="8"/>
       <c r="V798" s="35" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="799" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34715,7 +34713,7 @@
         <v>382</v>
       </c>
       <c r="N806" s="35" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="O806" s="7"/>
       <c r="P806" s="8" t="s">
@@ -34726,7 +34724,7 @@
       <c r="S806" s="8"/>
       <c r="T806" s="8"/>
       <c r="V806" s="35" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="807" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34760,7 +34758,7 @@
       <c r="S807" s="8"/>
       <c r="T807" s="8"/>
       <c r="V807" s="35" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="808" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35006,7 +35004,7 @@
       <c r="S815" s="8"/>
       <c r="T815" s="8"/>
       <c r="V815" s="35" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="816" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35341,7 +35339,7 @@
     </row>
     <row r="827" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A827" s="8" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="I827" s="38" t="s">
         <v>35</v>
@@ -35362,7 +35360,7 @@
         <v>403</v>
       </c>
       <c r="N827" s="35" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="O827" s="7"/>
       <c r="P827" s="8" t="s">
@@ -35373,7 +35371,7 @@
       <c r="S827" s="8"/>
       <c r="T827" s="8"/>
       <c r="V827" s="35" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="828" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35765,7 +35763,7 @@
       <c r="S840" s="8"/>
       <c r="T840" s="8"/>
       <c r="V840" s="35" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="841" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35829,7 +35827,7 @@
       <c r="S842" s="8"/>
       <c r="T842" s="8"/>
       <c r="V842" s="35" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="843" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35925,7 +35923,7 @@
         <v>163</v>
       </c>
       <c r="T845" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V845" s="35"/>
     </row>
@@ -36113,7 +36111,7 @@
         <v>119</v>
       </c>
       <c r="T851" s="8" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="V851" s="35"/>
     </row>
@@ -36148,7 +36146,7 @@
       <c r="S852" s="8"/>
       <c r="T852" s="8"/>
       <c r="V852" s="35" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="853" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36662,7 +36660,7 @@
       <c r="S869" s="8"/>
       <c r="T869" s="8"/>
       <c r="V869" s="35" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="870" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37634,7 +37632,7 @@
         <v>119</v>
       </c>
       <c r="T901" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V901" s="35"/>
     </row>
@@ -37762,7 +37760,7 @@
         <v>119</v>
       </c>
       <c r="T905" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V905" s="35"/>
     </row>
@@ -37892,7 +37890,7 @@
         <v>119</v>
       </c>
       <c r="T909" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V909" s="35"/>
     </row>
@@ -38019,7 +38017,7 @@
         <v>119</v>
       </c>
       <c r="T913" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V913" s="35"/>
     </row>
@@ -38143,7 +38141,7 @@
         <v>119</v>
       </c>
       <c r="T917" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V917" s="35"/>
     </row>
@@ -38477,7 +38475,7 @@
       <c r="S928" s="8"/>
       <c r="T928" s="8"/>
       <c r="V928" s="35" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="929" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38635,7 +38633,7 @@
       <c r="S933" s="8"/>
       <c r="T933" s="8"/>
       <c r="V933" s="35" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="934" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38859,10 +38857,10 @@
       <c r="Q940" s="8"/>
       <c r="R940" s="8"/>
       <c r="S940" s="8" t="s">
+        <v>1692</v>
+      </c>
+      <c r="T940" s="8" t="s">
         <v>1693</v>
-      </c>
-      <c r="T940" s="8" t="s">
-        <v>1694</v>
       </c>
       <c r="V940" s="35"/>
     </row>
@@ -38936,7 +38934,7 @@
       <c r="S942" s="8"/>
       <c r="T942" s="8"/>
       <c r="V942" s="35" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="943" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39669,7 +39667,7 @@
       <c r="S966" s="8"/>
       <c r="T966" s="8"/>
       <c r="V966" s="35" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="967" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40490,7 +40488,7 @@
       <c r="S992" s="8"/>
       <c r="T992" s="8"/>
       <c r="V992" s="35" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="993" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40948,7 +40946,7 @@
       <c r="S1006" s="8"/>
       <c r="T1006" s="8"/>
       <c r="V1006" s="35" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1007" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41244,7 +41242,7 @@
       <c r="S1015" s="8"/>
       <c r="T1015" s="8"/>
       <c r="V1015" s="35" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1016" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41466,7 +41464,7 @@
       <c r="S1022" s="8"/>
       <c r="T1022" s="8"/>
       <c r="V1022" s="35" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1023" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41746,7 +41744,7 @@
       <c r="S1031" s="8"/>
       <c r="T1031" s="8"/>
       <c r="V1031" s="35" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1032" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42178,7 +42176,7 @@
       <c r="S1045" s="8"/>
       <c r="T1045" s="8"/>
       <c r="V1045" s="35" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1046" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43079,7 +43077,7 @@
       <c r="S1074" s="8"/>
       <c r="T1074" s="8"/>
       <c r="V1074" s="35" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1075" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43514,7 +43512,7 @@
       <c r="S1088" s="8"/>
       <c r="T1088" s="8"/>
       <c r="V1088" s="35" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1089" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44321,7 +44319,7 @@
       <c r="S1114" s="8"/>
       <c r="T1114" s="8"/>
       <c r="V1114" s="35" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1115" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44385,7 +44383,7 @@
       <c r="S1116" s="8"/>
       <c r="T1116" s="8"/>
       <c r="V1116" s="35" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1117" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44510,7 +44508,7 @@
       <c r="S1120" s="8"/>
       <c r="T1120" s="8"/>
       <c r="V1120" s="35" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1121" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44545,7 +44543,7 @@
       <c r="S1121" s="8"/>
       <c r="T1121" s="8"/>
       <c r="V1121" s="35" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1122" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44613,7 +44611,7 @@
       <c r="S1123" s="8"/>
       <c r="T1123" s="8"/>
       <c r="V1123" s="35" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1124" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44650,7 +44648,7 @@
       <c r="S1124" s="8"/>
       <c r="T1124" s="8"/>
       <c r="V1124" s="35" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1125" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44687,7 +44685,7 @@
       <c r="S1125" s="8"/>
       <c r="T1125" s="8"/>
       <c r="V1125" s="35" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1126" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44821,7 +44819,7 @@
         <v>106</v>
       </c>
       <c r="T1129" s="8" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="V1129" s="35"/>
     </row>
@@ -45157,7 +45155,7 @@
       <c r="S1139" s="8"/>
       <c r="T1139" s="8"/>
       <c r="V1139" s="35" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1140" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45322,7 +45320,7 @@
         <v>106</v>
       </c>
       <c r="T1144" s="8" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="V1144" s="35"/>
     </row>
@@ -45390,12 +45388,12 @@
       <c r="S1146" s="8"/>
       <c r="T1146" s="8"/>
       <c r="V1146" s="35" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1147" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1147" s="55" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="H1147" s="42" t="s">
         <v>108</v>
@@ -45419,7 +45417,7 @@
         <v>320</v>
       </c>
       <c r="N1147" s="56" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="O1147" s="8" t="s">
         <v>78</v>
@@ -45430,7 +45428,7 @@
       <c r="S1147" s="8"/>
       <c r="T1147" s="8"/>
       <c r="V1147" s="35" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1148" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45496,7 +45494,7 @@
       <c r="S1149" s="8"/>
       <c r="T1149" s="8"/>
       <c r="V1149" s="35" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1150" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46193,7 +46191,7 @@
     </row>
     <row r="1172" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1172" s="8" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="I1172" s="38" t="s">
         <v>42</v>
@@ -46225,7 +46223,7 @@
       <c r="S1172" s="8"/>
       <c r="T1172" s="8"/>
       <c r="V1172" s="35" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1173" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46377,7 +46375,7 @@
       <c r="S1177" s="8"/>
       <c r="T1177" s="8"/>
       <c r="V1177" s="35" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1178" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47353,7 +47351,7 @@
       <c r="S1209" s="8"/>
       <c r="T1209" s="8"/>
       <c r="V1209" s="35" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1210" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47477,7 +47475,7 @@
       <c r="S1213" s="8"/>
       <c r="T1213" s="8"/>
       <c r="V1213" s="35" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1214" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48174,7 +48172,7 @@
         <v>119</v>
       </c>
       <c r="T1236" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V1236" s="35"/>
     </row>
@@ -48238,7 +48236,7 @@
         <v>119</v>
       </c>
       <c r="T1238" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1238" s="35"/>
     </row>
@@ -48663,7 +48661,7 @@
       <c r="S1252" s="8"/>
       <c r="T1252" s="8"/>
       <c r="V1252" s="35" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1253" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48851,7 +48849,7 @@
       <c r="S1258" s="8"/>
       <c r="T1258" s="8"/>
       <c r="V1258" s="35" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1259" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48885,7 +48883,7 @@
       <c r="S1259" s="8"/>
       <c r="T1259" s="8"/>
       <c r="V1259" s="35" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48919,7 +48917,7 @@
       <c r="S1260" s="8"/>
       <c r="T1260" s="8"/>
       <c r="V1260" s="35" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1261" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48953,7 +48951,7 @@
       <c r="S1261" s="8"/>
       <c r="T1261" s="8"/>
       <c r="V1261" s="35" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1262" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49139,7 +49137,7 @@
       <c r="S1267" s="8"/>
       <c r="T1267" s="8"/>
       <c r="V1267" s="35" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1268" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49268,7 +49266,7 @@
       <c r="S1271" s="8"/>
       <c r="T1271" s="8"/>
       <c r="V1271" s="35" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1272" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49302,7 +49300,7 @@
       <c r="S1272" s="8"/>
       <c r="T1272" s="8"/>
       <c r="V1272" s="35" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1273" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49335,7 +49333,7 @@
       <c r="S1273" s="8"/>
       <c r="T1273" s="8"/>
       <c r="V1273" s="35" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1274" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49905,7 +49903,7 @@
       <c r="S1291" s="8"/>
       <c r="T1291" s="8"/>
       <c r="U1291" s="8" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="V1291" s="35"/>
     </row>
@@ -50009,7 +50007,7 @@
       <c r="S1294" s="8"/>
       <c r="T1294" s="8"/>
       <c r="V1294" s="35" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1295" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50073,7 +50071,7 @@
       <c r="S1296" s="8"/>
       <c r="T1296" s="8"/>
       <c r="V1296" s="35" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1297" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50096,7 +50094,7 @@
         <v>125</v>
       </c>
       <c r="N1297" s="35" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="O1297" s="8" t="s">
         <v>78</v>
@@ -50109,7 +50107,7 @@
       <c r="S1297" s="8"/>
       <c r="T1297" s="8"/>
       <c r="V1297" s="35" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="1298" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50286,7 +50284,7 @@
         <v>131</v>
       </c>
       <c r="N1303" s="35" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="O1303" s="7"/>
       <c r="P1303" s="8" t="s">
@@ -50297,7 +50295,7 @@
       <c r="S1303" s="8"/>
       <c r="T1303" s="8"/>
       <c r="V1303" s="35" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1304" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50582,7 +50580,7 @@
       <c r="S1312" s="8"/>
       <c r="T1312" s="8"/>
       <c r="V1312" s="35" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="1313" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50617,7 +50615,7 @@
       <c r="S1313" s="8"/>
       <c r="T1313" s="8"/>
       <c r="V1313" s="35" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1314" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50796,7 +50794,7 @@
         <v>147</v>
       </c>
       <c r="N1319" s="35" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="O1319" s="7"/>
       <c r="P1319" s="8" t="s">
@@ -50807,7 +50805,7 @@
       <c r="S1319" s="8"/>
       <c r="T1319" s="8"/>
       <c r="V1319" s="35" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="1320" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50997,7 +50995,7 @@
       <c r="S1325" s="8"/>
       <c r="T1325" s="8"/>
       <c r="V1325" s="35" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1326" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51058,7 +51056,7 @@
         <v>155</v>
       </c>
       <c r="N1327" s="35" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="O1327" s="8"/>
       <c r="P1327" s="8" t="s">
@@ -51069,7 +51067,7 @@
       <c r="S1327" s="8"/>
       <c r="T1327" s="8"/>
       <c r="V1327" s="35" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1328" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51306,7 +51304,7 @@
       <c r="S1334" s="8"/>
       <c r="T1334" s="8"/>
       <c r="V1334" s="35" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1335" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52123,7 +52121,7 @@
       <c r="S1360" s="8"/>
       <c r="T1360" s="8"/>
       <c r="V1360" s="35" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1361" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52267,7 +52265,7 @@
       <c r="S1364" s="8"/>
       <c r="T1364" s="8"/>
       <c r="V1364" s="35" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1365" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52775,7 +52773,7 @@
       <c r="S1380" s="8"/>
       <c r="T1380" s="8"/>
       <c r="V1380" s="35" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1381" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53340,7 +53338,7 @@
       <c r="S1398" s="8"/>
       <c r="T1398" s="8"/>
       <c r="V1398" s="35" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53375,7 +53373,7 @@
       <c r="S1399" s="8"/>
       <c r="T1399" s="8"/>
       <c r="V1399" s="35" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1400" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53473,7 +53471,7 @@
       <c r="S1402" s="8"/>
       <c r="T1402" s="8"/>
       <c r="V1402" s="36" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1403" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53763,7 +53761,7 @@
       <c r="S1411" s="8"/>
       <c r="T1411" s="8"/>
       <c r="V1411" s="35" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1412" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53835,7 +53833,7 @@
       <c r="S1413" s="8"/>
       <c r="T1413" s="8"/>
       <c r="V1413" s="35" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1414" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54163,7 +54161,7 @@
       <c r="S1423" s="8"/>
       <c r="T1423" s="8"/>
       <c r="V1423" s="35" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1424" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54477,7 +54475,7 @@
       <c r="S1433" s="8"/>
       <c r="T1433" s="8"/>
       <c r="V1433" s="35" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1434" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54605,7 +54603,7 @@
       <c r="S1437" s="8"/>
       <c r="T1437" s="8"/>
       <c r="V1437" s="35" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1438" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54671,7 +54669,7 @@
       <c r="S1439" s="8"/>
       <c r="T1439" s="8"/>
       <c r="V1439" s="35" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1440" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54737,7 +54735,7 @@
       <c r="S1441" s="8"/>
       <c r="T1441" s="8"/>
       <c r="V1441" s="35" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1442" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54896,7 +54894,7 @@
       <c r="S1446" s="8"/>
       <c r="T1446" s="8"/>
       <c r="V1446" s="35" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1447" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55024,7 +55022,7 @@
       <c r="S1450" s="8"/>
       <c r="T1450" s="8"/>
       <c r="V1450" s="35" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1451" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55351,7 +55349,7 @@
       <c r="S1460" s="11"/>
       <c r="T1460" s="11"/>
       <c r="V1460" s="35" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1461" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55796,7 +55794,7 @@
     </row>
     <row r="1475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1475" s="8" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="C1475" s="30"/>
       <c r="H1475" s="26"/>
@@ -55830,7 +55828,7 @@
       <c r="S1475" s="8"/>
       <c r="T1475" s="8"/>
       <c r="V1475" s="35" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1476" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55896,7 +55894,7 @@
       <c r="S1477" s="8"/>
       <c r="T1477" s="8"/>
       <c r="V1477" s="35" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1478" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55932,7 +55930,7 @@
       <c r="S1478" s="8"/>
       <c r="T1478" s="8"/>
       <c r="V1478" s="35" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1479" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56094,7 +56092,7 @@
       <c r="S1483" s="8"/>
       <c r="T1483" s="8"/>
       <c r="V1483" s="35" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1484" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56160,7 +56158,7 @@
       <c r="S1485" s="8"/>
       <c r="T1485" s="8"/>
       <c r="V1485" s="35" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1486" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56224,10 +56222,10 @@
       <c r="Q1487" s="8"/>
       <c r="R1487" s="8"/>
       <c r="S1487" s="8" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="T1487" s="8" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="V1487" s="35"/>
     </row>
@@ -56327,7 +56325,7 @@
       <c r="S1490" s="8"/>
       <c r="T1490" s="8"/>
       <c r="V1490" s="35" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1491" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56455,7 +56453,7 @@
       <c r="S1494" s="8"/>
       <c r="T1494" s="8"/>
       <c r="V1494" s="35" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1495" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56510,7 +56508,7 @@
         <v>21</v>
       </c>
       <c r="N1496" s="35" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="O1496" s="7"/>
       <c r="P1496" s="8" t="s">
@@ -56521,7 +56519,7 @@
       <c r="S1496" s="8"/>
       <c r="T1496" s="8"/>
       <c r="V1496" s="35" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1497" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56593,7 +56591,7 @@
       <c r="S1498" s="8"/>
       <c r="T1498" s="8"/>
       <c r="V1498" s="35" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1499" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56797,7 +56795,7 @@
       <c r="S1504" s="8"/>
       <c r="T1504" s="8"/>
       <c r="V1504" s="35" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1505" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56821,7 +56819,7 @@
         <v>30</v>
       </c>
       <c r="N1505" s="35" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="O1505" s="8" t="s">
         <v>78</v>
@@ -56834,7 +56832,7 @@
       <c r="S1505" s="8"/>
       <c r="T1505" s="8"/>
       <c r="V1505" s="35" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1506" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56869,7 +56867,7 @@
       <c r="S1506" s="8"/>
       <c r="T1506" s="8"/>
       <c r="V1506" s="35" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1507" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56904,7 +56902,7 @@
       <c r="S1507" s="8"/>
       <c r="T1507" s="8"/>
       <c r="V1507" s="35" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1508" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57119,7 +57117,7 @@
         <v>39</v>
       </c>
       <c r="N1514" s="35" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="O1514" s="8" t="s">
         <v>78</v>
@@ -57132,7 +57130,7 @@
       <c r="S1514" s="8"/>
       <c r="T1514" s="8"/>
       <c r="V1514" s="35" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1515" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57251,7 +57249,7 @@
         <v>43</v>
       </c>
       <c r="N1518" s="35" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="O1518" s="8" t="s">
         <v>78</v>
@@ -57262,7 +57260,7 @@
       <c r="S1518" s="8"/>
       <c r="T1518" s="8"/>
       <c r="V1518" s="35" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1519" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57328,7 +57326,7 @@
       <c r="S1520" s="8"/>
       <c r="T1520" s="8"/>
       <c r="V1520" s="35" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1521" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57425,7 +57423,7 @@
       <c r="S1523" s="8"/>
       <c r="T1523" s="8"/>
       <c r="V1523" s="35" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1524" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57491,7 +57489,7 @@
       <c r="S1525" s="8"/>
       <c r="T1525" s="8"/>
       <c r="V1525" s="35" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1526" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57525,7 +57523,7 @@
       <c r="S1526" s="8"/>
       <c r="T1526" s="8"/>
       <c r="V1526" s="35" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1527" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57560,7 +57558,7 @@
       <c r="S1527" s="8"/>
       <c r="T1527" s="8"/>
       <c r="V1527" s="35" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1528" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57595,7 +57593,7 @@
       <c r="S1528" s="8"/>
       <c r="T1528" s="8"/>
       <c r="V1528" s="35" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1529" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57704,7 +57702,7 @@
       <c r="S1531" s="8"/>
       <c r="T1531" s="8"/>
       <c r="V1531" s="35" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="1532" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58018,7 +58016,7 @@
       <c r="S1541" s="8"/>
       <c r="T1541" s="8"/>
       <c r="V1541" s="35" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1542" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58041,7 +58039,7 @@
         <v>67</v>
       </c>
       <c r="N1542" s="35" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="O1542" s="7"/>
       <c r="P1542" s="8" t="s">
@@ -58052,7 +58050,7 @@
       <c r="S1542" s="8"/>
       <c r="T1542" s="8"/>
       <c r="V1542" s="35" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="1543" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58137,7 +58135,7 @@
       <c r="S1544" s="8"/>
       <c r="T1544" s="8"/>
       <c r="V1544" s="35" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1545" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58212,7 +58210,7 @@
       <c r="S1546" s="8"/>
       <c r="T1546" s="8"/>
       <c r="V1546" s="35" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1547" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58355,7 +58353,7 @@
         <v>76</v>
       </c>
       <c r="N1551" s="35" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="O1551" s="7"/>
       <c r="P1551" s="8" t="s">
@@ -58366,7 +58364,7 @@
       <c r="S1551" s="8"/>
       <c r="T1551" s="8"/>
       <c r="V1551" s="35" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1552" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58400,7 +58398,7 @@
       <c r="S1552" s="8"/>
       <c r="T1552" s="8"/>
       <c r="V1552" s="35" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1553" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58434,7 +58432,7 @@
       <c r="S1553" s="8"/>
       <c r="T1553" s="8"/>
       <c r="V1553" s="35" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1554" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58547,7 +58545,7 @@
         <v>82</v>
       </c>
       <c r="N1557" s="35" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="O1557" s="7"/>
       <c r="P1557" s="8" t="s">
@@ -58558,7 +58556,7 @@
       <c r="S1557" s="8"/>
       <c r="T1557" s="8"/>
       <c r="V1557" s="35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1558" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58741,7 +58739,7 @@
         <v>119</v>
       </c>
       <c r="T1563" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1563" s="35"/>
     </row>
@@ -58795,7 +58793,7 @@
         <v>90</v>
       </c>
       <c r="N1565" s="35" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="O1565" s="7"/>
       <c r="P1565" s="8" t="s">
@@ -58806,7 +58804,7 @@
       <c r="S1565" s="8"/>
       <c r="T1565" s="8"/>
       <c r="V1565" s="35" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1566" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58931,7 +58929,7 @@
       <c r="S1569" s="8"/>
       <c r="T1569" s="8"/>
       <c r="V1569" s="35" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1570" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59085,7 +59083,7 @@
       <c r="S1574" s="8"/>
       <c r="T1574" s="8"/>
       <c r="V1574" s="35" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1575" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59178,7 +59176,7 @@
       <c r="S1577" s="8"/>
       <c r="T1577" s="8"/>
       <c r="V1577" s="35" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1578" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59211,7 +59209,7 @@
         <v>119</v>
       </c>
       <c r="T1578" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1578" s="35"/>
     </row>
@@ -59289,13 +59287,13 @@
         <v>106</v>
       </c>
       <c r="N1581" s="35" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="P1581" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1581" s="35" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1582" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59477,7 +59475,7 @@
         <v>112</v>
       </c>
       <c r="N1587" s="35" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="O1587" s="8" t="s">
         <v>78</v>
@@ -59486,7 +59484,7 @@
         <v>79</v>
       </c>
       <c r="V1587" s="35" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1588" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59635,7 +59633,7 @@
         <v>119</v>
       </c>
       <c r="T1593" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1593" s="35"/>
     </row>
@@ -59683,13 +59681,13 @@
         <v>120</v>
       </c>
       <c r="N1595" s="35" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="P1595" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1595" s="35" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1596" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59865,13 +59863,13 @@
         <v>127</v>
       </c>
       <c r="N1602" s="35" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="P1602" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1602" s="35" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1603" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60020,7 +60018,7 @@
         <v>119</v>
       </c>
       <c r="T1608" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1608" s="35"/>
     </row>
@@ -60068,13 +60066,13 @@
         <v>135</v>
       </c>
       <c r="N1610" s="35" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="P1610" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1610" s="35" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1611" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60160,7 +60158,7 @@
         <v>78</v>
       </c>
       <c r="V1613" s="35" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1614" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60255,7 +60253,7 @@
         <v>142</v>
       </c>
       <c r="N1617" s="35" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="O1617" s="8" t="s">
         <v>78</v>
@@ -60264,7 +60262,7 @@
         <v>79</v>
       </c>
       <c r="V1617" s="35" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1618" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60413,7 +60411,7 @@
         <v>119</v>
       </c>
       <c r="T1623" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1623" s="35"/>
     </row>
@@ -60461,13 +60459,13 @@
         <v>150</v>
       </c>
       <c r="N1625" s="35" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="P1625" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1625" s="35" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1626" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60544,7 +60542,7 @@
         <v>78</v>
       </c>
       <c r="V1628" s="35" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1629" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60645,7 +60643,7 @@
         <v>79</v>
       </c>
       <c r="V1632" s="35" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1633" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60722,7 +60720,7 @@
         <v>78</v>
       </c>
       <c r="V1635" s="35" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1636" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60751,7 +60749,7 @@
         <v>119</v>
       </c>
       <c r="T1636" s="8" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="V1636" s="35"/>
     </row>
@@ -60805,7 +60803,7 @@
     </row>
     <row r="1639" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1639" s="8" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="I1639" s="38" t="s">
         <v>51</v>
@@ -60826,13 +60824,13 @@
         <v>164</v>
       </c>
       <c r="N1639" s="35" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="P1639" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1639" s="35" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1640" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60934,7 +60932,7 @@
         <v>78</v>
       </c>
       <c r="V1643" s="35" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1644" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61053,13 +61051,13 @@
         <v>9</v>
       </c>
       <c r="N1648" s="36" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="O1648" s="8" t="s">
         <v>78</v>
       </c>
       <c r="V1648" s="35" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1649" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61106,7 +61104,7 @@
         <v>11</v>
       </c>
       <c r="N1650" s="35" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="P1650" s="8" t="s">
         <v>79</v>
@@ -61115,7 +61113,7 @@
         <v>129</v>
       </c>
       <c r="V1650" s="35" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1651" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61378,7 +61376,7 @@
         <v>110</v>
       </c>
       <c r="V1660" s="35" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1661" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61407,7 +61405,7 @@
         <v>78</v>
       </c>
       <c r="V1661" s="35" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1662" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61859,7 +61857,7 @@
         <v>78</v>
       </c>
       <c r="V1679" s="35" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1680" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61966,7 +61964,7 @@
         <v>119</v>
       </c>
       <c r="T1683" s="8" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="V1683" s="35"/>
     </row>
@@ -62113,7 +62111,7 @@
         <v>78</v>
       </c>
       <c r="V1688" s="35" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1689" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62306,13 +62304,13 @@
         <v>57</v>
       </c>
       <c r="N1696" s="35" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="O1696" s="8" t="s">
         <v>78</v>
       </c>
       <c r="V1696" s="35" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="1697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62812,7 +62810,7 @@
         <v>79</v>
       </c>
       <c r="V1716" s="35" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1717" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62913,7 +62911,7 @@
         <v>78</v>
       </c>
       <c r="V1720" s="35" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1721" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62966,7 +62964,7 @@
         <v>78</v>
       </c>
       <c r="V1722" s="35" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1723" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63022,7 +63020,7 @@
         <v>79</v>
       </c>
       <c r="V1724" s="35" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1725" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63643,7 +63641,7 @@
         <v>78</v>
       </c>
       <c r="V1749" s="35" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1750" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63773,7 +63771,7 @@
         <v>78</v>
       </c>
       <c r="V1754" s="35" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1755" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63826,7 +63824,7 @@
         <v>78</v>
       </c>
       <c r="V1756" s="35" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1757" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63879,7 +63877,7 @@
         <v>78</v>
       </c>
       <c r="V1758" s="35" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1759" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64028,7 +64026,7 @@
         <v>78</v>
       </c>
       <c r="V1764" s="35" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1765" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64129,7 +64127,7 @@
         <v>78</v>
       </c>
       <c r="V1768" s="35" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1769" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64283,7 +64281,7 @@
         <v>78</v>
       </c>
       <c r="V1774" s="35" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1775" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64509,7 +64507,7 @@
         <v>78</v>
       </c>
       <c r="V1783" s="35" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1784" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64929,7 +64927,7 @@
         <v>78</v>
       </c>
       <c r="V1799" s="35" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65006,7 +65004,7 @@
         <v>78</v>
       </c>
       <c r="V1802" s="35" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1803" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65035,7 +65033,7 @@
         <v>78</v>
       </c>
       <c r="V1803" s="35" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1804" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65064,7 +65062,7 @@
         <v>78</v>
       </c>
       <c r="V1804" s="35" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1805" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65093,7 +65091,7 @@
         <v>79</v>
       </c>
       <c r="V1805" s="35" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="1806" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65151,7 +65149,7 @@
     </row>
     <row r="1808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1808" s="8" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="G1808" s="46" t="s">
         <v>153</v>
@@ -65187,7 +65185,7 @@
     </row>
     <row r="1809" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1809" s="8" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="G1809" s="46" t="s">
         <v>153</v>
@@ -65223,7 +65221,7 @@
     </row>
     <row r="1810" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1810" s="8" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="G1810" s="46" t="s">
         <v>153</v>
@@ -65310,7 +65308,7 @@
         <v>78</v>
       </c>
       <c r="V1812" s="35" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1813" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65333,7 +65331,7 @@
         <v>8</v>
       </c>
       <c r="N1813" s="35" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="O1813" s="8" t="s">
         <v>78</v>
@@ -65342,7 +65340,7 @@
         <v>79</v>
       </c>
       <c r="V1813" s="35" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1814" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65562,7 +65560,7 @@
         <v>17</v>
       </c>
       <c r="N1822" s="35" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="O1822" s="8" t="s">
         <v>78</v>
@@ -65571,7 +65569,7 @@
         <v>79</v>
       </c>
       <c r="V1822" s="35" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1823" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65702,7 +65700,7 @@
         <v>78</v>
       </c>
       <c r="V1827" s="35" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1828" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65823,7 +65821,7 @@
         <v>26</v>
       </c>
       <c r="N1831" s="35" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="O1831" s="8" t="s">
         <v>78</v>
@@ -65834,7 +65832,7 @@
       <c r="S1831" s="8"/>
       <c r="T1831" s="8"/>
       <c r="V1831" s="35" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1832" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66079,7 +66077,7 @@
         <v>78</v>
       </c>
       <c r="V1840" s="35" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1841" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66129,13 +66127,13 @@
         <v>37</v>
       </c>
       <c r="N1842" s="35" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="P1842" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V1842" s="35" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="1843" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66610,7 +66608,7 @@
     </row>
     <row r="1862" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1862" s="8" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I1862" s="38" t="s">
         <v>56</v>
@@ -66715,7 +66713,7 @@
         <v>78</v>
       </c>
       <c r="V1865" s="35" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1866" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66840,7 +66838,7 @@
     </row>
     <row r="1871" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1871" s="8" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="I1871" s="38" t="s">
         <v>56</v>
@@ -66870,7 +66868,7 @@
     </row>
     <row r="1872" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1872" s="8" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="I1872" s="38" t="s">
         <v>56</v>
@@ -67559,7 +67557,7 @@
         <v>78</v>
       </c>
       <c r="V1898" s="35" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1899" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67708,7 +67706,7 @@
         <v>78</v>
       </c>
       <c r="V1904" s="35" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1905" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67737,7 +67735,7 @@
         <v>78</v>
       </c>
       <c r="V1905" s="35" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1906" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68397,7 +68395,7 @@
         <v>78</v>
       </c>
       <c r="V1932" s="35" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1933" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68642,7 +68640,7 @@
         <v>78</v>
       </c>
       <c r="V1942" s="35" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1943" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69107,7 +69105,7 @@
         <v>78</v>
       </c>
       <c r="V1961" s="35" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1962" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69624,7 +69622,7 @@
         <v>78</v>
       </c>
       <c r="V1982" s="35" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1983" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69701,7 +69699,7 @@
         <v>78</v>
       </c>
       <c r="V1985" s="35" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1986" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70072,7 +70070,7 @@
         <v>78</v>
       </c>
       <c r="V2000" s="35" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="2001" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70250,7 +70248,7 @@
         <v>78</v>
       </c>
       <c r="V2007" s="35" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="2008" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70423,7 +70421,7 @@
         <v>78</v>
       </c>
       <c r="V2014" s="35" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="2015" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70820,7 +70818,7 @@
         <v>225</v>
       </c>
       <c r="N2030" s="35" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="O2030" s="8" t="s">
         <v>78</v>
@@ -70829,7 +70827,7 @@
         <v>79</v>
       </c>
       <c r="V2030" s="35" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="2031" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71446,7 +71444,7 @@
         <v>23</v>
       </c>
       <c r="N2053" s="36" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="V2053" s="35"/>
     </row>
@@ -71650,7 +71648,7 @@
         <v>31</v>
       </c>
       <c r="N2061" s="36" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="V2061" s="35"/>
     </row>
@@ -72025,7 +72023,7 @@
         <v>78</v>
       </c>
       <c r="V2076" s="35" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2077" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72154,7 +72152,7 @@
         <v>78</v>
       </c>
       <c r="V2081" s="35" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="2082" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72255,7 +72253,7 @@
         <v>78</v>
       </c>
       <c r="V2085" s="35" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="2086" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72356,7 +72354,7 @@
         <v>78</v>
       </c>
       <c r="V2089" s="35" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2090" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72409,7 +72407,7 @@
         <v>78</v>
       </c>
       <c r="V2091" s="35" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2092" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72611,10 +72609,10 @@
         <v>989</v>
       </c>
       <c r="S2099" s="8" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="T2099" s="8" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="V2099" s="35"/>
     </row>
@@ -72868,7 +72866,7 @@
         <v>78</v>
       </c>
       <c r="V2109" s="35" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="2110" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72948,7 +72946,7 @@
         <v>78</v>
       </c>
       <c r="V2112" s="35" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="2113" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73265,7 +73263,7 @@
         <v>78</v>
       </c>
       <c r="V2125" s="36" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2126" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73461,7 +73459,7 @@
         <v>78</v>
       </c>
       <c r="V2133" s="35" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="2134" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73514,7 +73512,7 @@
         <v>78</v>
       </c>
       <c r="V2135" s="35" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2136" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74317,7 +74315,7 @@
         <v>78</v>
       </c>
       <c r="V2168" s="35" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="2169" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74613,13 +74611,13 @@
         <v>150</v>
       </c>
       <c r="N2180" s="35" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="P2180" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2180" s="35" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="2181" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74814,7 +74812,7 @@
         <v>78</v>
       </c>
       <c r="V2188" s="35" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="2189" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75035,7 +75033,7 @@
         <v>78</v>
       </c>
       <c r="V2197" s="35" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2198" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75088,7 +75086,7 @@
         <v>78</v>
       </c>
       <c r="V2199" s="35" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2200" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75159,7 +75157,7 @@
         <v>22</v>
       </c>
       <c r="N2202" s="35" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="O2202" s="8" t="s">
         <v>78</v>
@@ -75168,7 +75166,7 @@
         <v>79</v>
       </c>
       <c r="V2202" s="35" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="2203" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75219,7 +75217,7 @@
         <v>78</v>
       </c>
       <c r="V2204" s="35" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2205" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75320,7 +75318,7 @@
         <v>78</v>
       </c>
       <c r="V2208" s="35" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2209" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75352,7 +75350,7 @@
         <v>78</v>
       </c>
       <c r="V2209" s="35" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="2210" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75465,7 +75463,7 @@
         <v>78</v>
       </c>
       <c r="V2213" s="35" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="2214" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75521,7 +75519,7 @@
         <v>78</v>
       </c>
       <c r="V2215" s="35" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="2216" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75550,7 +75548,7 @@
         <v>78</v>
       </c>
       <c r="V2216" s="35" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="2217" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75627,7 +75625,7 @@
         <v>78</v>
       </c>
       <c r="V2219" s="35" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="2220" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75656,7 +75654,7 @@
         <v>82</v>
       </c>
       <c r="V2220" s="35" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="2221" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75685,7 +75683,7 @@
         <v>78</v>
       </c>
       <c r="V2221" s="35" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="2222" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75714,7 +75712,7 @@
         <v>78</v>
       </c>
       <c r="V2222" s="35" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="2223" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75833,7 +75831,7 @@
         <v>25</v>
       </c>
       <c r="N2227" s="35" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="O2227" s="8" t="s">
         <v>78</v>
@@ -75842,7 +75840,7 @@
         <v>79</v>
       </c>
       <c r="V2227" s="35" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="2228" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76085,7 +76083,7 @@
         <v>78</v>
       </c>
       <c r="V2237" s="35" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="2238" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76186,7 +76184,7 @@
         <v>78</v>
       </c>
       <c r="V2241" s="35" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="2242" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76239,7 +76237,7 @@
         <v>78</v>
       </c>
       <c r="V2243" s="35" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="2244" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76364,7 +76362,7 @@
         <v>78</v>
       </c>
       <c r="V2248" s="35" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="2249" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76393,7 +76391,7 @@
         <v>78</v>
       </c>
       <c r="V2249" s="35" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="2250" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76422,7 +76420,7 @@
         <v>79</v>
       </c>
       <c r="V2250" s="35" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="2251" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76521,7 +76519,7 @@
         <v>78</v>
       </c>
       <c r="V2254" s="35" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="2255" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76598,7 +76596,7 @@
         <v>78</v>
       </c>
       <c r="V2257" s="35" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="2258" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76627,7 +76625,7 @@
         <v>78</v>
       </c>
       <c r="V2258" s="35" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="2259" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76656,7 +76654,7 @@
         <v>78</v>
       </c>
       <c r="V2259" s="35" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="2260" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76709,7 +76707,7 @@
         <v>78</v>
       </c>
       <c r="V2261" s="35" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="2262" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76834,7 +76832,7 @@
         <v>78</v>
       </c>
       <c r="V2266" s="35" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="2267" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76911,7 +76909,7 @@
         <v>78</v>
       </c>
       <c r="V2269" s="35" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="2270" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76964,13 +76962,13 @@
         <v>21</v>
       </c>
       <c r="N2271" s="35" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="P2271" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2271" s="35" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="2272" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76997,7 +76995,7 @@
         <v>78</v>
       </c>
       <c r="V2272" s="35" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="2273" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77026,7 +77024,7 @@
         <v>78</v>
       </c>
       <c r="V2273" s="35" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="2274" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77055,7 +77053,7 @@
         <v>82</v>
       </c>
       <c r="V2274" s="35" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="2275" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77108,7 +77106,7 @@
         <v>82</v>
       </c>
       <c r="V2276" s="35" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="2277" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77137,7 +77135,7 @@
         <v>78</v>
       </c>
       <c r="V2277" s="35" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="2278" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77160,7 +77158,7 @@
         <v>7</v>
       </c>
       <c r="N2278" s="35" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="O2278" s="8" t="s">
         <v>82</v>
@@ -77195,7 +77193,7 @@
         <v>78</v>
       </c>
       <c r="V2279" s="35" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77464,7 +77462,7 @@
         <v>78</v>
       </c>
       <c r="V2290" s="35" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="2291" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77517,7 +77515,7 @@
         <v>78</v>
       </c>
       <c r="V2292" s="35" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="2293" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77540,13 +77538,13 @@
         <v>22</v>
       </c>
       <c r="N2293" s="35" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="P2293" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2293" s="35" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="2294" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77747,7 +77745,7 @@
         <v>78</v>
       </c>
       <c r="V2301" s="35" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="2302" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77992,7 +77990,7 @@
         <v>78</v>
       </c>
       <c r="V2311" s="35" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="2312" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78069,7 +78067,7 @@
     </row>
     <row r="2315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2315" s="8" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="I2315" s="38" t="s">
         <v>67</v>
@@ -78090,13 +78088,13 @@
         <v>22</v>
       </c>
       <c r="N2315" s="35" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="P2315" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2315" s="35" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="2316" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78171,7 +78169,7 @@
         <v>78</v>
       </c>
       <c r="V2318" s="35" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="2319" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78200,7 +78198,7 @@
         <v>78</v>
       </c>
       <c r="V2319" s="35" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="2320" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78301,7 +78299,7 @@
         <v>78</v>
       </c>
       <c r="V2323" s="35" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="2324" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78690,7 +78688,7 @@
         <v>79</v>
       </c>
       <c r="V2339" s="35" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="2340" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78765,7 +78763,7 @@
         <v>78</v>
       </c>
       <c r="V2342" s="35" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="2343" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78794,7 +78792,7 @@
         <v>78</v>
       </c>
       <c r="V2343" s="35" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="2344" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78847,7 +78845,7 @@
         <v>78</v>
       </c>
       <c r="V2345" s="35" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78924,7 +78922,7 @@
         <v>78</v>
       </c>
       <c r="V2348" s="35" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="2349" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78977,7 +78975,7 @@
         <v>78</v>
       </c>
       <c r="V2350" s="35" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="2351" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79030,7 +79028,7 @@
         <v>78</v>
       </c>
       <c r="V2352" s="35" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="2353" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79202,13 +79200,13 @@
         <v>20</v>
       </c>
       <c r="N2359" s="35" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="P2359" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2359" s="35" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="2360" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79235,7 +79233,7 @@
         <v>78</v>
       </c>
       <c r="V2360" s="35" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="2361" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79312,7 +79310,7 @@
         <v>78</v>
       </c>
       <c r="V2363" s="35" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="2364" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79365,7 +79363,7 @@
         <v>78</v>
       </c>
       <c r="V2365" s="35" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="2366" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79394,7 +79392,7 @@
         <v>78</v>
       </c>
       <c r="V2366" s="35" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="2367" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79423,7 +79421,7 @@
         <v>78</v>
       </c>
       <c r="V2367" s="35" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="2368" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79452,7 +79450,7 @@
         <v>78</v>
       </c>
       <c r="V2368" s="35" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="2369" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79505,7 +79503,7 @@
         <v>78</v>
       </c>
       <c r="V2370" s="35" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="2371" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79558,7 +79556,7 @@
         <v>78</v>
       </c>
       <c r="V2372" s="35" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79611,7 +79609,7 @@
         <v>78</v>
       </c>
       <c r="V2374" s="35" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="2375" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79634,13 +79632,13 @@
         <v>16</v>
       </c>
       <c r="N2375" s="35" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="P2375" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2375" s="35" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="2376" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79667,7 +79665,7 @@
         <v>119</v>
       </c>
       <c r="T2376" s="8" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="V2376" s="35"/>
     </row>
@@ -79961,7 +79959,7 @@
         <v>78</v>
       </c>
       <c r="V2388" s="35" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="2389" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80086,7 +80084,7 @@
         <v>78</v>
       </c>
       <c r="V2393" s="35" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="2394" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80217,7 +80215,7 @@
         <v>78</v>
       </c>
       <c r="V2398" s="35" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="2399" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80273,7 +80271,7 @@
         <v>78</v>
       </c>
       <c r="V2400" s="35" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="2401" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80350,7 +80348,7 @@
         <v>79</v>
       </c>
       <c r="V2403" s="35" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="2404" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80449,7 +80447,7 @@
         <v>78</v>
       </c>
       <c r="V2407" s="35" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="2408" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80987,7 +80985,7 @@
         <v>78</v>
       </c>
       <c r="V2429" s="35" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="2430" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81058,13 +81056,13 @@
         <v>29</v>
       </c>
       <c r="N2432" s="35" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="P2432" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2432" s="35" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="2433" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81163,7 +81161,7 @@
         <v>78</v>
       </c>
       <c r="V2436" s="35" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="2437" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81684,7 +81682,7 @@
         <v>78</v>
       </c>
       <c r="V2457" s="35" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="2458" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81737,7 +81735,7 @@
     </row>
     <row r="2460" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2460" s="8" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="I2460" s="38" t="s">
         <v>73</v>
@@ -81758,13 +81756,13 @@
         <v>28</v>
       </c>
       <c r="N2460" s="35" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="P2460" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2460" s="35" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="2461" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81815,7 +81813,7 @@
         <v>78</v>
       </c>
       <c r="V2462" s="35" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="2463" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81844,7 +81842,7 @@
         <v>78</v>
       </c>
       <c r="V2463" s="35" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="2464" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82017,7 +82015,7 @@
         <v>78</v>
       </c>
       <c r="V2470" s="35" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="2471" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82070,7 +82068,7 @@
         <v>78</v>
       </c>
       <c r="V2472" s="35" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="2473" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82171,7 +82169,7 @@
         <v>78</v>
       </c>
       <c r="V2476" s="35" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="2477" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82224,7 +82222,7 @@
         <v>78</v>
       </c>
       <c r="V2478" s="35" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="2479" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82277,7 +82275,7 @@
         <v>78</v>
       </c>
       <c r="V2480" s="35" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="2481" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82324,7 +82322,7 @@
         <v>22</v>
       </c>
       <c r="N2482" s="35" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="O2482" s="8" t="s">
         <v>78</v>
@@ -82333,7 +82331,7 @@
         <v>79</v>
       </c>
       <c r="V2482" s="35" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="2483" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82525,7 +82523,7 @@
         <v>8</v>
       </c>
       <c r="N2490" s="35" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="O2490" s="8" t="s">
         <v>78</v>
@@ -82534,7 +82532,7 @@
         <v>79</v>
       </c>
       <c r="V2490" s="35" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="2491" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82635,7 +82633,7 @@
         <v>78</v>
       </c>
       <c r="V2494" s="35" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="2495" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82760,7 +82758,7 @@
         <v>78</v>
       </c>
       <c r="V2499" s="35" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="2500" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82783,13 +82781,13 @@
         <v>18</v>
       </c>
       <c r="N2500" s="35" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="P2500" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2500" s="35" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="2501" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82912,7 +82910,7 @@
         <v>78</v>
       </c>
       <c r="V2505" s="35" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="2506" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83151,7 +83149,7 @@
         <v>78</v>
       </c>
       <c r="V2514" s="35" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="2515" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83424,13 +83422,13 @@
         <v>25</v>
       </c>
       <c r="N2525" s="35" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="P2525" s="8" t="s">
         <v>79</v>
       </c>
       <c r="V2525" s="35" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="2526" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -84300,7 +84298,7 @@
         <v>119</v>
       </c>
       <c r="T2561" s="8" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="V2561" s="35"/>
     </row>
@@ -84402,7 +84400,7 @@
         <v>78</v>
       </c>
       <c r="V2565" s="35" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="2566" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -84842,7 +84840,7 @@
         <v>79</v>
       </c>
       <c r="V2583" s="35" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="2584" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 08 08 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE6F50D-F542-49A5-9A8F-63264AEC9ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4AD706-BC99-4352-B1BD-DA8E93B78330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4956,9 +4956,6 @@
     <t>rucaq itiq ruca#H</t>
   </si>
   <si>
-    <t>bRuqhaqspaqteq iti# bRuhaspate</t>
-  </si>
-  <si>
     <t>rucaqmitiq ruca$m</t>
   </si>
   <si>
@@ -5191,6 +5188,9 @@
   </si>
   <si>
     <t>eqte ityeqte</t>
+  </si>
+  <si>
+    <t>bRuqhaqspaqtaq iti# bRuhaspate</t>
   </si>
 </sst>
 </file>
@@ -5843,10 +5843,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1304" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U553" sqref="U553"/>
+      <selection pane="bottomLeft" activeCell="V1311" sqref="V1311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -12104,7 +12104,7 @@
         <v>119</v>
       </c>
       <c r="T154" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="U154" s="8"/>
       <c r="V154" s="35"/>
@@ -12518,7 +12518,7 @@
         <v>17</v>
       </c>
       <c r="N166" s="35" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="O166" s="7"/>
       <c r="P166" s="8" t="s">
@@ -14933,7 +14933,7 @@
         <v>83</v>
       </c>
       <c r="N232" s="36" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="O232" s="8" t="s">
         <v>78</v>
@@ -15805,7 +15805,7 @@
         <v>108</v>
       </c>
       <c r="N257" s="36" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="O257" s="8" t="s">
         <v>78</v>
@@ -20383,10 +20383,10 @@
       <c r="Q385" s="8"/>
       <c r="R385" s="8"/>
       <c r="S385" s="8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="T385" s="8" t="s">
         <v>1682</v>
-      </c>
-      <c r="T385" s="8" t="s">
-        <v>1683</v>
       </c>
       <c r="U385" s="8"/>
       <c r="V385" s="35"/>
@@ -21071,7 +21071,7 @@
         <v>255</v>
       </c>
       <c r="N404" s="36" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="O404" s="8" t="s">
         <v>78</v>
@@ -22783,7 +22783,7 @@
         <v>106</v>
       </c>
       <c r="T452" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="U452" s="8"/>
       <c r="V452" s="35"/>
@@ -25965,7 +25965,7 @@
       <c r="T542" s="8"/>
       <c r="U542" s="8"/>
       <c r="V542" s="36" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="543" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27378,7 +27378,7 @@
         <v>106</v>
       </c>
       <c r="T583" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="U583" s="8"/>
       <c r="V583" s="35"/>
@@ -28306,10 +28306,10 @@
       <c r="Q610" s="8"/>
       <c r="R610" s="8"/>
       <c r="S610" s="8" t="s">
+        <v>1685</v>
+      </c>
+      <c r="T610" s="8" t="s">
         <v>1686</v>
-      </c>
-      <c r="T610" s="8" t="s">
-        <v>1687</v>
       </c>
       <c r="U610" s="8"/>
       <c r="V610" s="35"/>
@@ -28625,7 +28625,7 @@
     </row>
     <row r="620" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A620" s="8" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B620" s="45"/>
       <c r="D620" s="17"/>
@@ -29084,7 +29084,7 @@
         <v>208</v>
       </c>
       <c r="N632" s="36" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="O632" s="8" t="s">
         <v>78</v>
@@ -29096,7 +29096,7 @@
       <c r="T632" s="8"/>
       <c r="U632" s="8"/>
       <c r="V632" s="36" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -31557,7 +31557,7 @@
     </row>
     <row r="708" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A708" s="8" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="G708" s="46" t="s">
         <v>152</v>
@@ -31596,7 +31596,7 @@
     </row>
     <row r="709" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A709" s="8" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="G709" s="46" t="s">
         <v>152</v>
@@ -33708,7 +33708,7 @@
         <v>351</v>
       </c>
       <c r="N775" s="36" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="O775" s="8" t="s">
         <v>78</v>
@@ -35339,7 +35339,7 @@
     </row>
     <row r="827" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A827" s="8" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="I827" s="38" t="s">
         <v>35</v>
@@ -35923,7 +35923,7 @@
         <v>163</v>
       </c>
       <c r="T845" s="8" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="V845" s="35"/>
     </row>
@@ -36111,7 +36111,7 @@
         <v>119</v>
       </c>
       <c r="T851" s="8" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="V851" s="35"/>
     </row>
@@ -37632,7 +37632,7 @@
         <v>119</v>
       </c>
       <c r="T901" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V901" s="35"/>
     </row>
@@ -37760,7 +37760,7 @@
         <v>119</v>
       </c>
       <c r="T905" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V905" s="35"/>
     </row>
@@ -37890,7 +37890,7 @@
         <v>119</v>
       </c>
       <c r="T909" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V909" s="35"/>
     </row>
@@ -38017,7 +38017,7 @@
         <v>119</v>
       </c>
       <c r="T913" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V913" s="35"/>
     </row>
@@ -38141,7 +38141,7 @@
         <v>119</v>
       </c>
       <c r="T917" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V917" s="35"/>
     </row>
@@ -38857,10 +38857,10 @@
       <c r="Q940" s="8"/>
       <c r="R940" s="8"/>
       <c r="S940" s="8" t="s">
+        <v>1691</v>
+      </c>
+      <c r="T940" s="8" t="s">
         <v>1692</v>
-      </c>
-      <c r="T940" s="8" t="s">
-        <v>1693</v>
       </c>
       <c r="V940" s="35"/>
     </row>
@@ -44819,7 +44819,7 @@
         <v>106</v>
       </c>
       <c r="T1129" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V1129" s="35"/>
     </row>
@@ -45320,7 +45320,7 @@
         <v>106</v>
       </c>
       <c r="T1144" s="8" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V1144" s="35"/>
     </row>
@@ -45393,7 +45393,7 @@
     </row>
     <row r="1147" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1147" s="55" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="H1147" s="42" t="s">
         <v>108</v>
@@ -45417,7 +45417,7 @@
         <v>320</v>
       </c>
       <c r="N1147" s="56" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="O1147" s="8" t="s">
         <v>78</v>
@@ -46191,7 +46191,7 @@
     </row>
     <row r="1172" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1172" s="8" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="I1172" s="38" t="s">
         <v>42</v>
@@ -48172,7 +48172,7 @@
         <v>119</v>
       </c>
       <c r="T1236" s="8" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V1236" s="35"/>
     </row>
@@ -48236,7 +48236,7 @@
         <v>119</v>
       </c>
       <c r="T1238" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1238" s="35"/>
     </row>
@@ -49903,7 +49903,7 @@
       <c r="S1291" s="8"/>
       <c r="T1291" s="8"/>
       <c r="U1291" s="8" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="V1291" s="35"/>
     </row>
@@ -50804,8 +50804,8 @@
       <c r="R1319" s="8"/>
       <c r="S1319" s="8"/>
       <c r="T1319" s="8"/>
-      <c r="V1319" s="35" t="s">
-        <v>1642</v>
+      <c r="V1319" s="36" t="s">
+        <v>1720</v>
       </c>
     </row>
     <row r="1320" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51304,7 +51304,7 @@
       <c r="S1334" s="8"/>
       <c r="T1334" s="8"/>
       <c r="V1334" s="35" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="1335" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55794,7 +55794,7 @@
     </row>
     <row r="1475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1475" s="8" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="C1475" s="30"/>
       <c r="H1475" s="26"/>
@@ -56158,7 +56158,7 @@
       <c r="S1485" s="8"/>
       <c r="T1485" s="8"/>
       <c r="V1485" s="35" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1486" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56222,10 +56222,10 @@
       <c r="Q1487" s="8"/>
       <c r="R1487" s="8"/>
       <c r="S1487" s="8" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="T1487" s="8" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="V1487" s="35"/>
     </row>
@@ -56519,7 +56519,7 @@
       <c r="S1496" s="8"/>
       <c r="T1496" s="8"/>
       <c r="V1496" s="35" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1497" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56832,7 +56832,7 @@
       <c r="S1505" s="8"/>
       <c r="T1505" s="8"/>
       <c r="V1505" s="35" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1506" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57423,7 +57423,7 @@
       <c r="S1523" s="8"/>
       <c r="T1523" s="8"/>
       <c r="V1523" s="35" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1524" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57702,7 +57702,7 @@
       <c r="S1531" s="8"/>
       <c r="T1531" s="8"/>
       <c r="V1531" s="35" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1532" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58050,7 +58050,7 @@
       <c r="S1542" s="8"/>
       <c r="T1542" s="8"/>
       <c r="V1542" s="35" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="1543" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58364,7 +58364,7 @@
       <c r="S1551" s="8"/>
       <c r="T1551" s="8"/>
       <c r="V1551" s="35" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="1552" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58556,7 +58556,7 @@
       <c r="S1557" s="8"/>
       <c r="T1557" s="8"/>
       <c r="V1557" s="35" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1558" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58739,7 +58739,7 @@
         <v>119</v>
       </c>
       <c r="T1563" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1563" s="35"/>
     </row>
@@ -58804,7 +58804,7 @@
       <c r="S1565" s="8"/>
       <c r="T1565" s="8"/>
       <c r="V1565" s="35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1566" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59083,7 +59083,7 @@
       <c r="S1574" s="8"/>
       <c r="T1574" s="8"/>
       <c r="V1574" s="35" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1575" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59209,7 +59209,7 @@
         <v>119</v>
       </c>
       <c r="T1578" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1578" s="35"/>
     </row>
@@ -59293,7 +59293,7 @@
         <v>79</v>
       </c>
       <c r="V1581" s="35" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1582" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59484,7 +59484,7 @@
         <v>79</v>
       </c>
       <c r="V1587" s="35" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1588" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59633,7 +59633,7 @@
         <v>119</v>
       </c>
       <c r="T1593" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1593" s="35"/>
     </row>
@@ -59687,7 +59687,7 @@
         <v>79</v>
       </c>
       <c r="V1595" s="35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1596" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59869,7 +59869,7 @@
         <v>79</v>
       </c>
       <c r="V1602" s="35" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1603" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60018,7 +60018,7 @@
         <v>119</v>
       </c>
       <c r="T1608" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1608" s="35"/>
     </row>
@@ -60072,7 +60072,7 @@
         <v>79</v>
       </c>
       <c r="V1610" s="35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1611" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60262,7 +60262,7 @@
         <v>79</v>
       </c>
       <c r="V1617" s="35" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1618" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60411,7 +60411,7 @@
         <v>119</v>
       </c>
       <c r="T1623" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1623" s="35"/>
     </row>
@@ -60465,7 +60465,7 @@
         <v>79</v>
       </c>
       <c r="V1625" s="35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1626" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60643,7 +60643,7 @@
         <v>79</v>
       </c>
       <c r="V1632" s="35" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1633" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60749,7 +60749,7 @@
         <v>119</v>
       </c>
       <c r="T1636" s="8" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V1636" s="35"/>
     </row>
@@ -60803,7 +60803,7 @@
     </row>
     <row r="1639" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1639" s="8" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="I1639" s="38" t="s">
         <v>51</v>
@@ -60830,7 +60830,7 @@
         <v>79</v>
       </c>
       <c r="V1639" s="35" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1640" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61051,7 +61051,7 @@
         <v>9</v>
       </c>
       <c r="N1648" s="36" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="O1648" s="8" t="s">
         <v>78</v>
@@ -61113,7 +61113,7 @@
         <v>129</v>
       </c>
       <c r="V1650" s="35" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1651" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61964,7 +61964,7 @@
         <v>119</v>
       </c>
       <c r="T1683" s="8" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="V1683" s="35"/>
     </row>
@@ -62304,13 +62304,13 @@
         <v>57</v>
       </c>
       <c r="N1696" s="35" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="O1696" s="8" t="s">
         <v>78</v>
       </c>
       <c r="V1696" s="35" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="1697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65091,7 +65091,7 @@
         <v>79</v>
       </c>
       <c r="V1805" s="35" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1806" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65149,7 +65149,7 @@
     </row>
     <row r="1808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1808" s="8" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G1808" s="46" t="s">
         <v>153</v>
@@ -65185,7 +65185,7 @@
     </row>
     <row r="1809" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1809" s="8" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="G1809" s="46" t="s">
         <v>153</v>
@@ -65221,7 +65221,7 @@
     </row>
     <row r="1810" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1810" s="8" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="G1810" s="46" t="s">
         <v>153</v>
@@ -65340,7 +65340,7 @@
         <v>79</v>
       </c>
       <c r="V1813" s="35" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="1814" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65569,7 +65569,7 @@
         <v>79</v>
       </c>
       <c r="V1822" s="35" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1823" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65832,7 +65832,7 @@
       <c r="S1831" s="8"/>
       <c r="T1831" s="8"/>
       <c r="V1831" s="35" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1832" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66133,7 +66133,7 @@
         <v>79</v>
       </c>
       <c r="V1842" s="35" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1843" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66608,7 +66608,7 @@
     </row>
     <row r="1862" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1862" s="8" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="I1862" s="38" t="s">
         <v>56</v>
@@ -66838,7 +66838,7 @@
     </row>
     <row r="1871" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1871" s="8" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="I1871" s="38" t="s">
         <v>56</v>
@@ -66868,7 +66868,7 @@
     </row>
     <row r="1872" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1872" s="8" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="I1872" s="38" t="s">
         <v>56</v>
@@ -70827,7 +70827,7 @@
         <v>79</v>
       </c>
       <c r="V2030" s="35" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="2031" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71444,7 +71444,7 @@
         <v>23</v>
       </c>
       <c r="N2053" s="36" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="V2053" s="35"/>
     </row>
@@ -71648,7 +71648,7 @@
         <v>31</v>
       </c>
       <c r="N2061" s="36" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="V2061" s="35"/>
     </row>
@@ -72609,10 +72609,10 @@
         <v>989</v>
       </c>
       <c r="S2099" s="8" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="T2099" s="8" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="V2099" s="35"/>
     </row>
@@ -74617,7 +74617,7 @@
         <v>79</v>
       </c>
       <c r="V2180" s="35" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="2181" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75166,7 +75166,7 @@
         <v>79</v>
       </c>
       <c r="V2202" s="35" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="2203" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75840,7 +75840,7 @@
         <v>79</v>
       </c>
       <c r="V2227" s="35" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="2228" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76420,7 +76420,7 @@
         <v>79</v>
       </c>
       <c r="V2250" s="35" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="2251" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76968,7 +76968,7 @@
         <v>79</v>
       </c>
       <c r="V2271" s="35" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="2272" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77158,7 +77158,7 @@
         <v>7</v>
       </c>
       <c r="N2278" s="35" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="O2278" s="8" t="s">
         <v>82</v>
@@ -77544,7 +77544,7 @@
         <v>79</v>
       </c>
       <c r="V2293" s="35" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="2294" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78067,7 +78067,7 @@
     </row>
     <row r="2315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2315" s="8" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="I2315" s="38" t="s">
         <v>67</v>
@@ -78094,7 +78094,7 @@
         <v>79</v>
       </c>
       <c r="V2315" s="35" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="2316" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79206,7 +79206,7 @@
         <v>79</v>
       </c>
       <c r="V2359" s="35" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="2360" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79638,7 +79638,7 @@
         <v>79</v>
       </c>
       <c r="V2375" s="35" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="2376" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79665,7 +79665,7 @@
         <v>119</v>
       </c>
       <c r="T2376" s="8" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="V2376" s="35"/>
     </row>
@@ -80348,7 +80348,7 @@
         <v>79</v>
       </c>
       <c r="V2403" s="35" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="2404" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81062,7 +81062,7 @@
         <v>79</v>
       </c>
       <c r="V2432" s="35" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="2433" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81735,7 +81735,7 @@
     </row>
     <row r="2460" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2460" s="8" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="I2460" s="38" t="s">
         <v>73</v>
@@ -81762,7 +81762,7 @@
         <v>79</v>
       </c>
       <c r="V2460" s="35" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="2461" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82331,7 +82331,7 @@
         <v>79</v>
       </c>
       <c r="V2482" s="35" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="2483" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82532,7 +82532,7 @@
         <v>79</v>
       </c>
       <c r="V2490" s="35" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="2491" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82787,7 +82787,7 @@
         <v>79</v>
       </c>
       <c r="V2500" s="35" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="2501" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83428,7 +83428,7 @@
         <v>79</v>
       </c>
       <c r="V2525" s="35" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="2526" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -84298,7 +84298,7 @@
         <v>119</v>
       </c>
       <c r="T2561" s="8" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="V2561" s="35"/>
     </row>

</xml_diff>

<commit_message>
nmv 09 08 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE1DA6-758E-494D-8AE8-11251E08529C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61877EA1-7E0B-444E-95ED-173CBF3296A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6661" uniqueCount="1721">
   <si>
     <t>Passage</t>
   </si>
@@ -5109,9 +5109,6 @@
     <t>S[r]+N[r]</t>
   </si>
   <si>
-    <t>svaqyaqmciH</t>
-  </si>
-  <si>
     <t>svaqyaqmciqtiriti# svayaM - ciqtiH</t>
   </si>
   <si>
@@ -5191,6 +5188,9 @@
   </si>
   <si>
     <t>sIqdaqteti# sIdata</t>
+  </si>
+  <si>
+    <t>svaqyaq~jciqtiH</t>
   </si>
 </sst>
 </file>
@@ -5843,10 +5843,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1598" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1721" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U1612" sqref="U1612"/>
+      <selection pane="bottomLeft" activeCell="U1737" sqref="U1737"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -14933,7 +14933,7 @@
         <v>83</v>
       </c>
       <c r="N232" s="36" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="O232" s="8" t="s">
         <v>78</v>
@@ -15805,7 +15805,7 @@
         <v>108</v>
       </c>
       <c r="N257" s="36" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="O257" s="8" t="s">
         <v>78</v>
@@ -21071,7 +21071,7 @@
         <v>255</v>
       </c>
       <c r="N404" s="36" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="O404" s="8" t="s">
         <v>78</v>
@@ -25965,7 +25965,7 @@
       <c r="T542" s="8"/>
       <c r="U542" s="8"/>
       <c r="V542" s="36" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="543" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28625,7 +28625,7 @@
     </row>
     <row r="620" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A620" s="8" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="B620" s="45"/>
       <c r="D620" s="17"/>
@@ -29084,7 +29084,7 @@
         <v>208</v>
       </c>
       <c r="N632" s="36" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="O632" s="8" t="s">
         <v>78</v>
@@ -29096,7 +29096,7 @@
       <c r="T632" s="8"/>
       <c r="U632" s="8"/>
       <c r="V632" s="36" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -33708,7 +33708,7 @@
         <v>351</v>
       </c>
       <c r="N775" s="36" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="O775" s="8" t="s">
         <v>78</v>
@@ -35339,7 +35339,7 @@
     </row>
     <row r="827" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A827" s="8" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="I827" s="38" t="s">
         <v>35</v>
@@ -45393,7 +45393,7 @@
     </row>
     <row r="1147" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1147" s="55" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="H1147" s="42" t="s">
         <v>108</v>
@@ -45417,7 +45417,7 @@
         <v>320</v>
       </c>
       <c r="N1147" s="56" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="O1147" s="8" t="s">
         <v>78</v>
@@ -46191,7 +46191,7 @@
     </row>
     <row r="1172" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1172" s="8" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I1172" s="38" t="s">
         <v>42</v>
@@ -50805,7 +50805,7 @@
       <c r="S1319" s="8"/>
       <c r="T1319" s="8"/>
       <c r="V1319" s="36" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="1320" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55794,7 +55794,7 @@
     </row>
     <row r="1475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1475" s="8" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="C1475" s="30"/>
       <c r="H1475" s="26"/>
@@ -57315,7 +57315,7 @@
         <v>45</v>
       </c>
       <c r="N1520" s="36" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="O1520" s="8" t="s">
         <v>78</v>
@@ -58364,7 +58364,7 @@
       <c r="S1551" s="8"/>
       <c r="T1551" s="8"/>
       <c r="V1551" s="36" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="1552" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60797,7 +60797,7 @@
     </row>
     <row r="1639" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1639" s="8" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="I1639" s="38" t="s">
         <v>51</v>
@@ -61045,7 +61045,7 @@
         <v>9</v>
       </c>
       <c r="N1648" s="36" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="O1648" s="8" t="s">
         <v>78</v>
@@ -62297,14 +62297,14 @@
         <f t="shared" si="81"/>
         <v>57</v>
       </c>
-      <c r="N1696" s="35" t="s">
-        <v>1693</v>
+      <c r="N1696" s="36" t="s">
+        <v>1720</v>
       </c>
       <c r="O1696" s="8" t="s">
         <v>78</v>
       </c>
       <c r="V1696" s="35" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="1697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62674,9 +62674,6 @@
       <c r="N1711" s="53" t="s">
         <v>888</v>
       </c>
-      <c r="U1711" s="8" t="s">
-        <v>128</v>
-      </c>
       <c r="V1711" s="35"/>
     </row>
     <row r="1712" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63337,9 +63334,6 @@
       </c>
       <c r="N1737" s="53" t="s">
         <v>888</v>
-      </c>
-      <c r="U1737" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="V1737" s="35"/>
     </row>
@@ -65143,7 +65137,7 @@
     </row>
     <row r="1808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1808" s="8" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="G1808" s="46" t="s">
         <v>153</v>
@@ -65179,7 +65173,7 @@
     </row>
     <row r="1809" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1809" s="8" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="G1809" s="46" t="s">
         <v>153</v>
@@ -65215,7 +65209,7 @@
     </row>
     <row r="1810" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1810" s="8" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="G1810" s="46" t="s">
         <v>153</v>
@@ -66602,7 +66596,7 @@
     </row>
     <row r="1862" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1862" s="8" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I1862" s="38" t="s">
         <v>56</v>
@@ -66832,7 +66826,7 @@
     </row>
     <row r="1871" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1871" s="8" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="I1871" s="38" t="s">
         <v>56</v>
@@ -66862,7 +66856,7 @@
     </row>
     <row r="1872" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1872" s="8" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="I1872" s="38" t="s">
         <v>56</v>
@@ -71438,7 +71432,7 @@
         <v>23</v>
       </c>
       <c r="N2053" s="36" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="V2053" s="35"/>
     </row>
@@ -71642,7 +71636,7 @@
         <v>31</v>
       </c>
       <c r="N2061" s="36" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="V2061" s="35"/>
     </row>
@@ -77152,7 +77146,7 @@
         <v>7</v>
       </c>
       <c r="N2278" s="35" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="O2278" s="8" t="s">
         <v>82</v>
@@ -78061,7 +78055,7 @@
     </row>
     <row r="2315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2315" s="8" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="I2315" s="38" t="s">
         <v>67</v>
@@ -81729,7 +81723,7 @@
     </row>
     <row r="2460" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2460" s="8" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="I2460" s="38" t="s">
         <v>73</v>

</xml_diff>